<commit_message>
OCL - Struttura Varianti
</commit_message>
<xml_diff>
--- a/File/Dati.xlsx
+++ b/File/Dati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgettiVbNet\stegip\ImpOrd\File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4F5FED-E23B-4659-B269-12F29A9860D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9524E7-672E-4A34-A651-339497281D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1B256489-4A08-493A-9882-1E10793A348E}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="75">
   <si>
     <t>cod.cliente</t>
   </si>
@@ -257,9 +257,6 @@
     <t>DataConsegna</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>T-SHIRT 190</t>
   </si>
   <si>
@@ -272,10 +269,25 @@
     <t>T-SHIRT 190 gr colore verde lime</t>
   </si>
   <si>
-    <t>Lavorazione1</t>
-  </si>
-  <si>
     <t>Lavorazione2</t>
+  </si>
+  <si>
+    <t>CODLAV1</t>
+  </si>
+  <si>
+    <t>TERZ1</t>
+  </si>
+  <si>
+    <t>CODLAV2</t>
+  </si>
+  <si>
+    <t>TERZ2</t>
+  </si>
+  <si>
+    <t>2 - S ; 10 - M ; 6 - L ; 2 - XL ; 15 - XXL ; 10 - XXXL ; 5 - XXXXL</t>
+  </si>
+  <si>
+    <t>B06</t>
   </si>
 </sst>
 </file>
@@ -356,7 +368,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,6 +384,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,7 +422,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -442,6 +472,32 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="2" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="2" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Euro" xfId="4" xr:uid="{73E2BE84-CC8E-4A4E-9FAE-56278F312163}"/>
@@ -762,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06BE478-2D65-44E7-924E-036C042382E0}">
   <dimension ref="A1:AZ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,11 +836,15 @@
     <col min="16" max="16" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="50.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21" style="35" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="35"/>
+    <col min="22" max="22" width="11.85546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.7109375" style="42" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.85546875" style="42" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="20.42578125" bestFit="1" customWidth="1"/>
@@ -816,7 +876,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="27" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -841,31 +901,29 @@
         <v>14</v>
       </c>
       <c r="P1" s="3"/>
-      <c r="Q1" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="Q1" s="28"/>
       <c r="R1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="37" t="s">
         <v>22</v>
       </c>
       <c r="Z1" s="4" t="s">
@@ -964,7 +1022,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>61</v>
@@ -978,9 +1036,7 @@
       <c r="I2" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="11" t="s">
-        <v>64</v>
-      </c>
+      <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="M2" s="12">
@@ -995,38 +1051,36 @@
       <c r="P2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="Q2" s="10" t="s">
-        <v>52</v>
-      </c>
+      <c r="Q2" s="10"/>
       <c r="R2" s="1">
         <v>1657</v>
       </c>
       <c r="S2" s="14">
         <v>4.8</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="U2" s="1">
-        <v>1</v>
-      </c>
-      <c r="V2" s="15">
-        <v>1</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="X2" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="15">
+      <c r="U2" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="V2" s="32">
+        <v>1</v>
+      </c>
+      <c r="W2" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="X2" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y2" s="39">
         <v>1</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>2</v>
+        <v>71</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="AB2" s="15">
         <v>1</v>
@@ -1122,16 +1176,20 @@
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="F3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
+      <c r="H3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>73</v>
+      </c>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
@@ -1142,10 +1200,10 @@
         <v>50</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="Q3" s="10"/>
       <c r="R3" s="1">
@@ -1154,22 +1212,22 @@
       <c r="S3" s="14">
         <v>4.8</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="U3" s="1">
-        <v>1</v>
-      </c>
-      <c r="V3" s="15">
+      <c r="T3" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="U3" s="31">
+        <v>1</v>
+      </c>
+      <c r="V3" s="32">
         <v>3</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="W3" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="X3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="15">
+      <c r="X3" s="38">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="39">
         <v>1</v>
       </c>
       <c r="Z3" s="1" t="s">
@@ -1280,12 +1338,12 @@
       <c r="Q4" s="23"/>
       <c r="R4" s="23"/>
       <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="23"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="23"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="40"/>
+      <c r="X4" s="40"/>
+      <c r="Y4" s="40"/>
       <c r="Z4" s="23"/>
       <c r="AA4" s="23"/>
       <c r="AB4" s="23"/>
@@ -1335,12 +1393,12 @@
       <c r="Q5" s="26"/>
       <c r="R5" s="26"/>
       <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="26"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="41"/>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="41"/>
       <c r="Z5" s="26"/>
       <c r="AA5" s="26"/>
       <c r="AB5" s="26"/>
@@ -1382,12 +1440,12 @@
       <c r="Q6" s="26"/>
       <c r="R6" s="26"/>
       <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
-      <c r="U6" s="26"/>
-      <c r="V6" s="26"/>
-      <c r="W6" s="26"/>
-      <c r="X6" s="26"/>
-      <c r="Y6" s="26"/>
+      <c r="T6" s="34"/>
+      <c r="U6" s="34"/>
+      <c r="V6" s="34"/>
+      <c r="W6" s="41"/>
+      <c r="X6" s="41"/>
+      <c r="Y6" s="41"/>
       <c r="Z6" s="26"/>
       <c r="AA6" s="26"/>
       <c r="AB6" s="26"/>
@@ -1429,12 +1487,12 @@
       <c r="Q7" s="26"/>
       <c r="R7" s="26"/>
       <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
-      <c r="V7" s="26"/>
-      <c r="W7" s="26"/>
-      <c r="X7" s="26"/>
-      <c r="Y7" s="26"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="34"/>
+      <c r="V7" s="34"/>
+      <c r="W7" s="41"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41"/>
       <c r="Z7" s="26"/>
       <c r="AA7" s="26"/>
       <c r="AB7" s="26"/>

</xml_diff>